<commit_message>
2.3.11: Enable type inference (abbreviation of type declaration) in TypeScript.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoCgFieldValueObject.xlsx
+++ b/meta/program/BlancoCgFieldValueObject.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoCg/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{880B4811-6BF4-0342-8E2B-7CD9072A928E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B06B0C9-58B2-C34D-B731-D401C08BC827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6740" yWindow="1460" windowWidth="28800" windowHeight="17540" tabRatio="640"/>
+    <workbookView xWindow="6740" yWindow="1460" windowWidth="28800" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -344,12 +344,32 @@
   </si>
   <si>
     <t>このフィールドにnullを与えられた際に引数例外を発生させるかどうか。</t>
+  </si>
+  <si>
+    <t>typeInference</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>型推論（型宣言の省略）をする場合はtrue</t>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">カタスイロｎ </t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">センゲンヲ </t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t xml:space="preserve">ショウリャク </t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -895,41 +915,41 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1268,14 +1288,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:F36"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1342,12 +1362,12 @@
         <v>12</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="55"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="51"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="17" t="s">
@@ -1448,23 +1468,23 @@
       <c r="F18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="59" t="s">
+      <c r="A19" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="57"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="54"/>
       <c r="F19"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="59"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="57"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="54"/>
       <c r="F20"/>
     </row>
     <row r="21" spans="1:6">
@@ -1501,29 +1521,29 @@
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A25" s="59" t="s">
+      <c r="A25" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="58" t="s">
+      <c r="C25" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="58" t="s">
+      <c r="D25" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="58" t="s">
+      <c r="E25" s="55" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="30"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="59"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
+      <c r="A26" s="56"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6">
@@ -1561,7 +1581,7 @@
     </row>
     <row r="29" spans="1:6" ht="30" customHeight="1">
       <c r="A29" s="44">
-        <f t="shared" ref="A29:A38" si="0">A28+1</f>
+        <f t="shared" ref="A29:A39" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="45" t="s">
@@ -1571,10 +1591,10 @@
         <v>38</v>
       </c>
       <c r="D29" s="46"/>
-      <c r="E29" s="50" t="s">
+      <c r="E29" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="51"/>
+      <c r="F29" s="53"/>
     </row>
     <row r="30" spans="1:6" ht="30" customHeight="1">
       <c r="A30" s="44">
@@ -1590,10 +1610,10 @@
       <c r="D30" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="E30" s="50" t="s">
+      <c r="E30" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="F30" s="51"/>
+      <c r="F30" s="53"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="44">
@@ -1685,10 +1705,10 @@
       <c r="D35" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="52" t="s">
+      <c r="E35" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="F35" s="51"/>
+      <c r="F35" s="53"/>
     </row>
     <row r="36" spans="1:6" ht="70.5" customHeight="1">
       <c r="A36" s="44">
@@ -1702,10 +1722,10 @@
         <v>35</v>
       </c>
       <c r="D36" s="46"/>
-      <c r="E36" s="50" t="s">
+      <c r="E36" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="F36" s="51"/>
+      <c r="F36" s="53"/>
     </row>
     <row r="37" spans="1:6" ht="27.75" customHeight="1">
       <c r="A37" s="44">
@@ -1721,10 +1741,10 @@
       <c r="D37" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="E37" s="50" t="s">
+      <c r="E37" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="F37" s="51"/>
+      <c r="F37" s="53"/>
     </row>
     <row r="38" spans="1:6" ht="85.5" customHeight="1">
       <c r="A38" s="44">
@@ -1738,29 +1758,49 @@
         <v>45</v>
       </c>
       <c r="D38" s="24"/>
-      <c r="E38" s="56" t="s">
+      <c r="E38" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="F38" s="51"/>
+      <c r="F38" s="53"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="22"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
+      <c r="A39" s="44">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="24" t="s">
+        <v>68</v>
+      </c>
       <c r="F39" s="25"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="26"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="29"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="25"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="26"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E35:F35"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="E19:E20"/>
@@ -1777,27 +1817,26 @@
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E35:F35"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D56">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D57" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>adjustDefaultValue</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>createToString</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>isAbstract</formula1>
     </dataValidation>
   </dataValidations>
@@ -1810,7 +1849,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>